<commit_message>
Committing before messing with bitbucket.
</commit_message>
<xml_diff>
--- a/DungeonsAndDragons/resources/GamalBattleCard.xlsx
+++ b/DungeonsAndDragons/resources/GamalBattleCard.xlsx
@@ -29,19 +29,400 @@
     <t>Gamal</t>
   </si>
   <si>
-    <t>Level 1 Leader</t>
-  </si>
-  <si>
     <t>Medium Deva Runepriest</t>
   </si>
   <si>
-    <t>+5 vs AC; 3 damage and the target is immobilized until the</t>
-  </si>
-  <si>
     <t>end of next turn or until I'm not adj to it.</t>
   </si>
   <si>
-    <t>attack to this target deals +3 damage.</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Word of Binding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (standard; at-will) - Weapon</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rune of Dest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Before the end of my next turn, the next</t>
+    </r>
+  </si>
+  <si>
+    <t>the end of my next turn.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Word of Exchange </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(standard; at-will) - Weapon</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Rune of Dest: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Before end of my next turn, the next attack</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rune of Prot: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Target takes -2 to all defenses until the end</t>
+    </r>
+  </si>
+  <si>
+    <t>of my next turn, and the next ally to hit the target by then</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Divine Rune of Thunder </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(standard; Encounter) - Weapon</t>
+    </r>
+  </si>
+  <si>
+    <t>combat advantage until the end of my next turn.</t>
+  </si>
+  <si>
+    <t>until the end of my next turn.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rune of the Undeniable Dawn </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(standard; Daily) - Weapon</t>
+    </r>
+  </si>
+  <si>
+    <t>my next turn. My allies and I gain a +2 to all defenses</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">while within the zone. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Sustain minor: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The zone persists.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Effect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The burst creates a zone that lasts until the end of</t>
+    </r>
+  </si>
+  <si>
+    <t>You or one ally within close burst 5</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rune of Dest: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>You and each ally in burst gain +2 to damage</t>
+    </r>
+  </si>
+  <si>
+    <t>rolls until the end of my next turn.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rune of Prot: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>You and each ally in burst gain +1 to all</t>
+    </r>
+  </si>
+  <si>
+    <t>defenses until the end of my next turn.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Memory of a Thousand Lifetimes </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(free; Encounter)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Trigger: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>You make an attack roll, a saving throw, a skill check,</t>
+    </r>
+  </si>
+  <si>
+    <t>or an ability check and dislike the result.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Effect: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I add 1d6 to the triggering roll.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alignment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Lawful Good</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Languages</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Common</t>
+    </r>
+  </si>
+  <si>
+    <t>Elven, Giant</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rune of Mending </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(minor; twice per encounter) </t>
+    </r>
+  </si>
+  <si>
+    <t>Target can spend a healing surge. Gains 1 temp hp also.</t>
+  </si>
+  <si>
+    <t>Level 2 Leader</t>
   </si>
   <si>
     <r>
@@ -63,7 +444,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> +1</t>
+      <t xml:space="preserve"> +2</t>
     </r>
   </si>
   <si>
@@ -86,7 +467,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Perception +3; normal vision</t>
+      <t xml:space="preserve"> Perception +4; normal vision</t>
     </r>
   </si>
   <si>
@@ -109,7 +490,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 25; </t>
+      <t xml:space="preserve"> 30; </t>
     </r>
     <r>
       <rPr>
@@ -130,7 +511,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 12</t>
+      <t xml:space="preserve"> 15</t>
     </r>
   </si>
   <si>
@@ -153,7 +534,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 11; </t>
+      <t xml:space="preserve"> 18; </t>
     </r>
     <r>
       <rPr>
@@ -174,7 +555,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 13; </t>
+      <t xml:space="preserve"> 14; </t>
     </r>
     <r>
       <rPr>
@@ -195,7 +576,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 11; </t>
+      <t xml:space="preserve"> 12; </t>
     </r>
     <r>
       <rPr>
@@ -216,7 +597,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 15</t>
+      <t xml:space="preserve"> 16</t>
     </r>
   </si>
   <si>
@@ -239,53 +620,228 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 6</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Word of Binding</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (standard; at-will) - Weapon</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Rune of Dest</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Before the end of my next turn, the next</t>
+      <t xml:space="preserve"> 5</t>
+    </r>
+  </si>
+  <si>
+    <t>+6 vs AC; 4 damage and the target is immobilized until the</t>
+  </si>
+  <si>
+    <t>attack to this target deals +4 damage.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rune of Prot: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 ally adj to me or tgt gains a +4 AC until</t>
+    </r>
+  </si>
+  <si>
+    <t>+6 vs AC; 1d8 +4 damage.</t>
+  </si>
+  <si>
+    <t>on this target from ally deals extra 4 damage and ally</t>
+  </si>
+  <si>
+    <t>gains 4 temporary hit points.</t>
+  </si>
+  <si>
+    <t>gains +4 AC until end of my next turn.</t>
+  </si>
+  <si>
+    <t>+6 vs AC; 1d8 + 4 thunder damage.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rune of Dest: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Add 4 to damage roll and the target grants</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Rune of Prot: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Push the target 4 squares, and it is dazed</t>
+    </r>
+  </si>
+  <si>
+    <t>+6 vs AC; Each enemy in close burst 3</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1d8 + 4 radiant damage. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Miss: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Half damage.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Skills</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2 acro, 7 arc, 4 ath, 1 blf, 1 dip, 4 dun, 2 end, 4 heal, 9 hist,</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9 ins, 1 int, 4 nat, 4 perc, 9 rel, 2 stl, 1str, 1 thv</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Str</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 16 (+4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dex</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 12 (+2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Wis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 16 (+4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Con</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 13 (+2)</t>
     </r>
   </si>
   <si>
@@ -308,545 +864,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 12 (+1)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rune of Prot: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1 ally adj to me or tgt gains a +3 AC until</t>
-    </r>
-  </si>
-  <si>
-    <t>the end of my next turn.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Word of Exchange </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(standard; at-will) - Weapon</t>
-    </r>
-  </si>
-  <si>
-    <t>+5 vs AC; 1d8 +3 damage.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Rune of Dest: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Before end of my next turn, the next attack</t>
-    </r>
-  </si>
-  <si>
-    <t>on this target from ally deals extra 3 damage and ally</t>
-  </si>
-  <si>
-    <t>gains 3 temporary hit points.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rune of Prot: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Target takes -2 to all defenses until the end</t>
-    </r>
-  </si>
-  <si>
-    <t>of my next turn, and the next ally to hit the target by then</t>
-  </si>
-  <si>
-    <t>gains +3 AC until end of my next turn.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Divine Rune of Thunder </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(standard; Encounter) - Weapon</t>
-    </r>
-  </si>
-  <si>
-    <t>+5 vs AC; 1d8 + 3 thunder damage.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rune of Dest: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Add 3 to damage roll and the target grants</t>
-    </r>
-  </si>
-  <si>
-    <t>combat advantage until the end of my next turn.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Rune of Prot: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Push the target 3 squares, and it is dazed</t>
-    </r>
-  </si>
-  <si>
-    <t>until the end of my next turn.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rune of the Undeniable Dawn </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(standard; Daily) - Weapon</t>
-    </r>
-  </si>
-  <si>
-    <t>+5 vs AC; Each enemy in close burst 3</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1d8 + 3 radiant damage. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Miss: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Half damage.</t>
-    </r>
-  </si>
-  <si>
-    <t>my next turn. My allies and I gain a +2 to all defenses</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">while within the zone. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Sustain minor: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The zone persists.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Effect</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: The burst creates a zone that lasts until the end of</t>
-    </r>
-  </si>
-  <si>
-    <t>You or one ally within close burst 5</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rune of Dest: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>You and each ally in burst gain +2 to damage</t>
-    </r>
-  </si>
-  <si>
-    <t>rolls until the end of my next turn.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rune of Prot: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>You and each ally in burst gain +1 to all</t>
-    </r>
-  </si>
-  <si>
-    <t>defenses until the end of my next turn.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Memory of a Thousand Lifetimes </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(free; Encounter)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Trigger: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>You make an attack roll, a saving throw, a skill check,</t>
-    </r>
-  </si>
-  <si>
-    <t>or an ability check and dislike the result.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Effect: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>I add 1d6 to the triggering roll.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alignment</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Lawful Good</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Languages</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Common</t>
-    </r>
-  </si>
-  <si>
-    <t>Elven, Giant</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Skills</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 1 acro, 6 arc, 3 ath, 3 dun, 1 end, 3 heal, 8 hist, 8 ins</t>
-    </r>
-  </si>
-  <si>
-    <t>3 nat, 3 perc, 8 rel, 1 stealth, 1 thievery</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Str</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 16 (+3)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Con</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 13 (+1)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Dex</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 12 (+1)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Wis</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 16 (+3)</t>
+      <t xml:space="preserve"> 12 (+2)</t>
     </r>
   </si>
   <si>
@@ -869,26 +887,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 11 (+0)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rune of Mending </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(minor; twice per encounter) </t>
-    </r>
-  </si>
-  <si>
-    <t>Target can spend a healing surge. Gains 1 temp hp also.</t>
+      <t xml:space="preserve"> 11 (+1)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1548,7 +1548,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1568,12 +1568,12 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1581,17 +1581,17 @@
     </row>
     <row r="3" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1599,7 +1599,7 @@
     </row>
     <row r="5" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="6" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1616,7 +1616,7 @@
     <row r="7" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -1624,7 +1624,7 @@
     <row r="8" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1632,7 +1632,7 @@
     <row r="9" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1640,7 +1640,7 @@
     <row r="10" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1648,7 +1648,7 @@
     <row r="11" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1656,7 +1656,7 @@
     <row r="12" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="7" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1664,14 +1664,14 @@
     <row r="13" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1679,7 +1679,7 @@
     <row r="15" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1687,7 +1687,7 @@
     <row r="16" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1695,7 +1695,7 @@
     <row r="17" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1703,7 +1703,7 @@
     <row r="18" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1711,7 +1711,7 @@
     <row r="19" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="7" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1719,7 +1719,7 @@
     <row r="20" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -1727,14 +1727,14 @@
     <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -1742,7 +1742,7 @@
     <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -1750,7 +1750,7 @@
     <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="7" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1758,7 +1758,7 @@
     <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="8" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -1766,7 +1766,7 @@
     <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="8" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -1774,14 +1774,14 @@
     <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="8" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="9" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -1789,7 +1789,7 @@
     <row r="29" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -1797,7 +1797,7 @@
     <row r="30" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="5" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1805,7 +1805,7 @@
     <row r="31" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="5" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -1813,7 +1813,7 @@
     <row r="32" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1821,7 +1821,7 @@
     <row r="33" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -1829,7 +1829,7 @@
     <row r="34" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="9" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -1837,7 +1837,7 @@
     <row r="35" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="5" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -1845,7 +1845,7 @@
     <row r="36" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="5" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -1853,7 +1853,7 @@
     <row r="37" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="7" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -1861,7 +1861,7 @@
     <row r="38" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="5" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -1869,7 +1869,7 @@
     <row r="39" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="7" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -1877,14 +1877,14 @@
     <row r="40" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="5" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1892,7 +1892,7 @@
     </row>
     <row r="42" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -1900,7 +1900,7 @@
     </row>
     <row r="43" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1908,7 +1908,7 @@
     </row>
     <row r="44" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -1916,12 +1916,12 @@
     </row>
     <row r="45" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -1929,12 +1929,12 @@
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -1943,14 +1943,14 @@
     <row r="48" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="4" t="s">
@@ -1962,14 +1962,14 @@
     </row>
     <row r="50" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="4" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>